<commit_message>
refactor: code and files structure
</commit_message>
<xml_diff>
--- a/WpfApp2/TEST.xlsx
+++ b/WpfApp2/TEST.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\profil_arkadiuszw\Desktop\dssmith 2021-01-22\Wpf_Sek20210121\WpfApp2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D0B5E45-38EC-49D4-9EDF-497D31B0D0B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{430FB29F-DA3E-4A4F-9886-EAEB44534ABC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5580" yWindow="2640" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -239,6 +239,74 @@
   </cellStyles>
   <dxfs count="12">
     <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
       <fill>
         <patternFill patternType="solid">
@@ -281,74 +349,6 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -466,11 +466,11 @@
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{03C6BBC9-965F-43B4-BFD8-171630148140}" name="MHA    " dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{7CD5C9A8-AB7A-4DE3-8E88-5BFD3218267E}" name="Rack    " dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{539B175C-0E12-4F49-9FD1-01B26FE5BBE0}" name="X-Coor    " dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{7CC59D85-547C-4A50-8FC9-DD9B0CC7253B}" name="Y-Coor" dataDxfId="0"/>
-    <tableColumn id="5" xr3:uid="{A8B52691-1130-4894-A486-A40E890D3ECC}" name="LocType    " dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{3C8CEE94-ABB4-4DC0-A21B-E58F4EC8F6CE}" name="CheckSum    " dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{8072B19A-09D8-4524-B895-2C75206F7070}" name="Zone    " dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{539B175C-0E12-4F49-9FD1-01B26FE5BBE0}" name="X-Coor    " dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{7CC59D85-547C-4A50-8FC9-DD9B0CC7253B}" name="Y-Coor" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{A8B52691-1130-4894-A486-A40E890D3ECC}" name="LocType    " dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{3C8CEE94-ABB4-4DC0-A21B-E58F4EC8F6CE}" name="CheckSum    " dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{8072B19A-09D8-4524-B895-2C75206F7070}" name="Zone    " dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -742,7 +742,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
feat: sending scripts by ethernet
</commit_message>
<xml_diff>
--- a/WpfApp2/TEST.xlsx
+++ b/WpfApp2/TEST.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\profil_arkadiuszw\Desktop\dssmith 2021-01-22\Wpf_Sek20210121\WpfApp2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{430FB29F-DA3E-4A4F-9886-EAEB44534ABC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB45DCDC-45C3-4EFA-AF45-790C39CA2FE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5580" yWindow="2640" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1008" yWindow="2808" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="15">
   <si>
     <t xml:space="preserve">MHA    </t>
   </si>
@@ -67,6 +67,9 @@
   </si>
   <si>
     <t>Y-Coor</t>
+  </si>
+  <si>
+    <t>Shelf</t>
   </si>
 </sst>
 </file>
@@ -219,7 +222,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -233,11 +236,21 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="13">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -461,16 +474,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B63628D2-7079-4FA3-B74A-F3BCC307B031}" name="Tabela1" displayName="Tabela1" ref="A1:G5" totalsRowShown="0" headerRowDxfId="11" dataDxfId="9" headerRowBorderDxfId="10" tableBorderDxfId="8" totalsRowBorderDxfId="7">
-  <autoFilter ref="A1:G5" xr:uid="{B63628D2-7079-4FA3-B74A-F3BCC307B031}"/>
-  <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{03C6BBC9-965F-43B4-BFD8-171630148140}" name="MHA    " dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{7CD5C9A8-AB7A-4DE3-8E88-5BFD3218267E}" name="Rack    " dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{539B175C-0E12-4F49-9FD1-01B26FE5BBE0}" name="X-Coor    " dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{7CC59D85-547C-4A50-8FC9-DD9B0CC7253B}" name="Y-Coor" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{A8B52691-1130-4894-A486-A40E890D3ECC}" name="LocType    " dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{3C8CEE94-ABB4-4DC0-A21B-E58F4EC8F6CE}" name="CheckSum    " dataDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{8072B19A-09D8-4524-B895-2C75206F7070}" name="Zone    " dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B63628D2-7079-4FA3-B74A-F3BCC307B031}" name="Tabela1" displayName="Tabela1" ref="A1:H5" totalsRowShown="0" headerRowDxfId="12" dataDxfId="10" headerRowBorderDxfId="11" tableBorderDxfId="9" totalsRowBorderDxfId="8">
+  <autoFilter ref="A1:H5" xr:uid="{B63628D2-7079-4FA3-B74A-F3BCC307B031}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{03C6BBC9-965F-43B4-BFD8-171630148140}" name="MHA    " dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{7CD5C9A8-AB7A-4DE3-8E88-5BFD3218267E}" name="Rack    " dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{539B175C-0E12-4F49-9FD1-01B26FE5BBE0}" name="X-Coor    " dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{7CC59D85-547C-4A50-8FC9-DD9B0CC7253B}" name="Y-Coor" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{A8B52691-1130-4894-A486-A40E890D3ECC}" name="LocType    " dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{3C8CEE94-ABB4-4DC0-A21B-E58F4EC8F6CE}" name="CheckSum    " dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{8072B19A-09D8-4524-B895-2C75206F7070}" name="Zone    " dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{680B283E-76F3-4A92-AD01-2A5362932C4A}" name="Shelf" dataDxfId="0">
+      <calculatedColumnFormula>RIGHT(Tabela1[[#This Row],[Y-Coor]], 1)</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -739,10 +755,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -753,7 +769,7 @@
     <col min="6" max="6" width="13.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -775,8 +791,11 @@
       <c r="G1" s="6" t="s">
         <v>5</v>
       </c>
+      <c r="H1" s="5" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -798,8 +817,12 @@
       <c r="G2" s="3" t="s">
         <v>8</v>
       </c>
+      <c r="H2" s="13" t="str">
+        <f>RIGHT(Tabela1[[#This Row],[Y-Coor]], 1)</f>
+        <v>1</v>
+      </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -821,8 +844,12 @@
       <c r="G3" s="3" t="s">
         <v>8</v>
       </c>
+      <c r="H3" s="13" t="str">
+        <f>RIGHT(Tabela1[[#This Row],[Y-Coor]], 1)</f>
+        <v>2</v>
+      </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>6</v>
       </c>
@@ -844,8 +871,12 @@
       <c r="G4" s="9" t="s">
         <v>8</v>
       </c>
+      <c r="H4" s="13" t="str">
+        <f>RIGHT(Tabela1[[#This Row],[Y-Coor]], 1)</f>
+        <v>3</v>
+      </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>6</v>
       </c>
@@ -866,6 +897,10 @@
       </c>
       <c r="G5" s="9" t="s">
         <v>8</v>
+      </c>
+      <c r="H5" s="13" t="str">
+        <f>RIGHT(Tabela1[[#This Row],[Y-Coor]], 1)</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>